<commit_message>
Working on fixing errors, writing more functions
</commit_message>
<xml_diff>
--- a/Tests/Excel/Test Data.xlsx
+++ b/Tests/Excel/Test Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IsaiahMartin\source\repos\Calcpad\Tests\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{393BF22B-FA3B-4508-945C-E062E96401F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BAB1312-ED73-4584-8B43-B57AD9B05884}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{EC660DEE-E84B-4C27-99E2-B7A3FCEBAAC4}"/>
   </bookViews>
@@ -645,7 +645,7 @@
   <dimension ref="A2:R29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+      <selection activeCell="G5" sqref="G5:G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>